<commit_message>
preliminary review of the schematic and layout
</commit_message>
<xml_diff>
--- a/Kiki/Deliverable Review.xlsx
+++ b/Kiki/Deliverable Review.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
   <si>
     <t>Author</t>
   </si>
@@ -143,6 +143,57 @@
   </si>
   <si>
     <t>Missing State: Cooldown? After the heater is turned off how does the user now when it is safe to open the kiln door and take out the tube?</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Schematic</t>
+  </si>
+  <si>
+    <t>1kohm limiting resistors on 7-segment display seems high. What is the current going through them</t>
+  </si>
+  <si>
+    <t>Can you drive the SCR directly from the Arduino pin. How much current does it draw? Will you overdrive the SCR if it connected directly to the pin? Is there are special drive circuitry needed to interface to the SCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the purpose of the 4.7kohm resistors on the transistor gates? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power indicator on 5V? You mentioned you wanted this but I do not see it. </t>
+  </si>
+  <si>
+    <t>SPI signals are mislabeld. The standard is SCK, MISO, MOSI, and CS</t>
+  </si>
+  <si>
+    <t>Make the color for LED1 an Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General: Value should be the part number for the component. If you want to add more information use the Attribute tool. Correct JP3. </t>
+  </si>
+  <si>
+    <t>Standard Reference Designator for Transistors  is "Q" not "T"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 5V signal connected to  JP3.9 should be connected to the 5V pin on the Arduino. The VIN pin is for when you want to power the Arduino off something other that the USB. </t>
+  </si>
+  <si>
+    <t>Consider making the bottom side of the board a ground plane. This will simplify your routing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can simplify the routing of the 7-Seg diplay by rotating it 180°. </t>
+  </si>
+  <si>
+    <t>The standard packade for resistors is 1206 not 603</t>
+  </si>
+  <si>
+    <t>for the 7-seg you do not need to show diemensions</t>
+  </si>
+  <si>
+    <t>For the spi traces if you come from the other side of the connector you will not have to change layers</t>
   </si>
 </sst>
 </file>
@@ -222,8 +273,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,7 +345,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -305,6 +362,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -321,6 +381,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -650,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1002,6 +1065,207 @@
         <v>37</v>
       </c>
     </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45">
+      <c r="A26">
+        <v>0.1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75">
+      <c r="A27">
+        <v>0.1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30">
+      <c r="A28">
+        <v>0.1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30">
+        <v>0.1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60">
+      <c r="A31">
+        <v>0.1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>0.1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30">
+      <c r="A33">
+        <v>0.1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60">
+      <c r="A34">
+        <v>0.1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45">
+      <c r="A35">
+        <v>0.1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30">
+      <c r="A36">
+        <v>0.1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30">
+      <c r="A37">
+        <v>0.1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30">
+      <c r="A38">
+        <v>0.1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45">
+      <c r="A39">
+        <v>0.1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
review of kiln schematic and layout
</commit_message>
<xml_diff>
--- a/Kiki/Deliverable Review.xlsx
+++ b/Kiki/Deliverable Review.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="456" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28520" windowHeight="17540" tabRatio="456"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>Author</t>
   </si>
@@ -240,16 +244,57 @@
   <si>
     <t>For the spi traces if you come from the other side of the connector you will not have to change layers</t>
   </si>
+  <si>
+    <t>See Feature_Block_Diagram V02 Comments.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Values for resistors and Capacitors are not displayed </t>
+  </si>
+  <si>
+    <t>Center Schemtic in middle of the frame</t>
+  </si>
+  <si>
+    <t>Find a frame that better matches the size of the circuit</t>
+  </si>
+  <si>
+    <t>Values not displayed on R1 - R11</t>
+  </si>
+  <si>
+    <t>Display Values</t>
+  </si>
+  <si>
+    <t>Thermocoule footprint has no component outline</t>
+  </si>
+  <si>
+    <t>Minor: Designer name and rev should be on the symbol layer not the net layer</t>
+  </si>
+  <si>
+    <t>Starter button not on schematic</t>
+  </si>
+  <si>
+    <t>Ready indicator not on schematic</t>
+  </si>
+  <si>
+    <t>Headers for arduino shield come off the botton of the board</t>
+  </si>
+  <si>
+    <t>PCB Milling</t>
+  </si>
+  <si>
+    <t>Closure</t>
+  </si>
+  <si>
+    <t>Move all traces on that connect to headers to the top side of the board</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -258,22 +303,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -288,7 +318,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -308,6 +338,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +356,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -326,150 +364,438 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.1953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.5023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.5023255813954"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8325581395349"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5348837209302"/>
+    <col min="2" max="2" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="36.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="16">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="4">
         <v>42635</v>
       </c>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="16">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="16">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -478,7 +804,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="16">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -489,7 +815,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" ht="32">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -510,11 +836,11 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="57.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B7" s="0" t="s">
+    <row r="7" spans="1:7" ht="60">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -530,11 +856,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -550,11 +876,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="1:7" ht="45">
+      <c r="A9">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -570,11 +896,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:7" ht="75">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -586,13 +912,12 @@
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B11" s="0" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="A11">
+        <v>0.1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -608,11 +933,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -628,11 +953,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:7" ht="45">
+      <c r="A13">
+        <v>0.1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -644,13 +969,12 @@
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B14" s="0" t="s">
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>0.1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -659,16 +983,15 @@
       <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>0.1</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -677,16 +1000,15 @@
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="0"/>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:7" ht="45">
+      <c r="A16">
+        <v>0.1</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -695,16 +1017,15 @@
       <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17">
+        <v>0.1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -720,11 +1041,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B18" s="0" t="s">
+    <row r="18" spans="1:6" ht="60">
+      <c r="A18">
+        <v>0.1</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -736,15 +1057,15 @@
       <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B19" s="0" t="s">
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19">
+        <v>0.1</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -753,16 +1074,15 @@
       <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B20" s="0" t="s">
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20">
+        <v>0.1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -771,31 +1091,29 @@
       <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B21" s="0" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="30">
+      <c r="A21">
+        <v>0.1</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22">
+        <v>0.1</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -804,34 +1122,20 @@
       <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B26" s="0" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="45">
+      <c r="A26">
+        <v>0.1</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -840,16 +1144,15 @@
       <c r="D26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="57.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B27" s="0" t="s">
+    <row r="27" spans="1:6" ht="90">
+      <c r="A27">
+        <v>0.1</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -858,16 +1161,15 @@
       <c r="D27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="1:6" ht="60">
+      <c r="A28">
+        <v>0.1</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -876,16 +1178,15 @@
       <c r="D28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="1:6" ht="30">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -894,16 +1195,15 @@
       <c r="D29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="0"/>
       <c r="F29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B30" s="0" t="s">
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30">
+        <v>0.1</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -912,16 +1212,15 @@
       <c r="D30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="0"/>
       <c r="F30" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B31" s="0" t="s">
+    <row r="31" spans="1:6" ht="60">
+      <c r="A31">
+        <v>0.1</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -930,16 +1229,15 @@
       <c r="D31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="0"/>
       <c r="F31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B32" s="0" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>0.1</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -948,16 +1246,15 @@
       <c r="D32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="0"/>
       <c r="F32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B33" s="0" t="s">
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33">
+        <v>0.1</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -966,16 +1263,15 @@
       <c r="D33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="0"/>
       <c r="F33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B34" s="0" t="s">
+    <row r="34" spans="1:6" ht="75">
+      <c r="A34">
+        <v>0.1</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -984,16 +1280,15 @@
       <c r="D34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="0"/>
       <c r="F34" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B35" s="0" t="s">
+    <row r="35" spans="1:6" ht="45">
+      <c r="A35">
+        <v>0.1</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1002,16 +1297,15 @@
       <c r="D35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="0"/>
       <c r="F35" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B36" s="0" t="s">
+    <row r="36" spans="1:6" ht="30">
+      <c r="A36">
+        <v>0.1</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1020,16 +1314,15 @@
       <c r="D36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="0"/>
       <c r="F36" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B37" s="0" t="s">
+    <row r="37" spans="1:6" ht="30">
+      <c r="A37">
+        <v>0.1</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1038,16 +1331,15 @@
       <c r="D37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="0"/>
       <c r="F37" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B38" s="0" t="s">
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38">
+        <v>0.1</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1056,16 +1348,15 @@
       <c r="D38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="0"/>
       <c r="F38" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B39" s="0" t="s">
+    <row r="39" spans="1:6" ht="45">
+      <c r="A39">
+        <v>0.1</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1074,21 +1365,176 @@
       <c r="D39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="0"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30">
+      <c r="A42">
+        <v>0.2</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>0.2</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>0.2</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>0.2</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30">
+      <c r="A46">
+        <v>0.2</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>0.2</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30">
+      <c r="A48">
+        <v>0.2</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49">
+        <v>0.2</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50">
+        <v>0.2</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53">
+        <v>0.2</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F27" r:id="rId1" display="http://www.americanmicrosemi.com/catalog/SC649000.html"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>